<commit_message>
Different disrupted agents with CASE setup
</commit_message>
<xml_diff>
--- a/Distributed/initialization/Conference Case - New.xlsx
+++ b/Distributed/initialization/Conference Case - New.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MBIA\MBIA_SCModeling\Distributed\initialization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PhD-UMich\BRGResearch\MBIA\Simulation\MBIA_MB\Distributed\initialization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23FB158-6BC9-4D19-8098-FAF345323B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29448711-9266-4912-9CF6-39B78369216D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-44378" yWindow="-1990" windowWidth="14033" windowHeight="15356" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00_SD" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -499,13 +499,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,20 +788,20 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="5" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="5" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -850,7 +848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -889,7 +887,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -928,7 +926,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -967,7 +965,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1006,7 +1004,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1045,7 +1043,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1084,7 +1082,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1162,7 +1160,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -1201,7 +1199,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -1240,7 +1238,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1279,7 +1277,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -1318,7 +1316,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1357,7 +1355,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -1396,7 +1394,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -1436,7 +1434,7 @@
       </c>
       <c r="P16" s="7"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1476,7 +1474,7 @@
       </c>
       <c r="P17" s="7"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1516,7 +1514,7 @@
       </c>
       <c r="P18" s="7"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1556,20 +1554,20 @@
       </c>
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="11">
-        <v>0</v>
-      </c>
-      <c r="D20" s="10">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10">
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9">
         <v>1</v>
       </c>
       <c r="F20" s="1">
@@ -1578,10 +1576,10 @@
       <c r="G20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="12">
         <v>247</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="12">
         <v>277.05</v>
       </c>
       <c r="J20" s="1">
@@ -1590,31 +1588,31 @@
       <c r="K20" s="5">
         <v>0.98</v>
       </c>
-      <c r="L20" s="10">
-        <v>0</v>
-      </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10">
+      <c r="L20" s="9">
+        <v>0</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9">
         <v>672</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9">
         <v>375</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="11">
-        <v>0</v>
-      </c>
-      <c r="D21" s="10">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10">
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
         <v>1</v>
       </c>
       <c r="F21" s="1">
@@ -1623,10 +1621,10 @@
       <c r="G21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="12">
         <v>106</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="12">
         <v>118.73</v>
       </c>
       <c r="J21" s="1">
@@ -1635,31 +1633,31 @@
       <c r="K21" s="5">
         <v>0.98</v>
       </c>
-      <c r="L21" s="10">
-        <v>0</v>
-      </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10">
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9">
         <v>672</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="9">
         <v>350</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="11">
-        <v>0</v>
-      </c>
-      <c r="D22" s="10">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
         <v>1</v>
       </c>
       <c r="F22" s="1">
@@ -1668,10 +1666,10 @@
       <c r="G22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="12">
         <v>193</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="12">
         <v>180.11</v>
       </c>
       <c r="J22" s="1">
@@ -1680,30 +1678,30 @@
       <c r="K22" s="5">
         <v>0.98</v>
       </c>
-      <c r="L22" s="10">
-        <v>0</v>
-      </c>
-      <c r="N22" s="10">
+      <c r="L22" s="9">
+        <v>0</v>
+      </c>
+      <c r="N22" s="9">
         <v>672</v>
       </c>
-      <c r="O22" s="10">
+      <c r="O22" s="9">
         <v>325</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="11">
-        <v>0</v>
-      </c>
-      <c r="D23" s="10">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10">
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
         <v>1</v>
       </c>
       <c r="F23" s="1">
@@ -1712,10 +1710,10 @@
       <c r="G23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="13">
         <v>289</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="12">
         <v>270.17</v>
       </c>
       <c r="J23" s="1">
@@ -1724,31 +1722,30 @@
       <c r="K23" s="5">
         <v>0.98</v>
       </c>
-      <c r="L23" s="10">
-        <v>0</v>
-      </c>
-      <c r="M23" s="12"/>
-      <c r="N23" s="10">
+      <c r="L23" s="9">
+        <v>0</v>
+      </c>
+      <c r="N23" s="9">
         <v>672</v>
       </c>
-      <c r="O23" s="10">
+      <c r="O23" s="9">
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="11">
-        <v>0</v>
-      </c>
-      <c r="D24" s="10">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10">
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
         <v>1</v>
       </c>
       <c r="F24" s="1">
@@ -1757,10 +1754,10 @@
       <c r="G24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="9">
         <v>1688</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="9">
         <v>1158.1400000000001</v>
       </c>
       <c r="J24" s="1">
@@ -1769,30 +1766,30 @@
       <c r="K24" s="5">
         <v>0.98</v>
       </c>
-      <c r="L24" s="10">
-        <v>0</v>
-      </c>
-      <c r="N24" s="10">
+      <c r="L24" s="9">
+        <v>0</v>
+      </c>
+      <c r="N24" s="9">
         <v>672</v>
       </c>
-      <c r="O24" s="10">
+      <c r="O24" s="9">
         <v>275</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="11">
-        <v>0</v>
-      </c>
-      <c r="D25" s="10">
-        <v>0</v>
-      </c>
-      <c r="E25" s="10">
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
         <v>1</v>
       </c>
       <c r="F25" s="1">
@@ -1801,10 +1798,10 @@
       <c r="G25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="9">
         <v>2062</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="9">
         <v>1415.49</v>
       </c>
       <c r="J25" s="1">
@@ -1813,30 +1810,30 @@
       <c r="K25" s="5">
         <v>0.98</v>
       </c>
-      <c r="L25" s="10">
-        <v>0</v>
-      </c>
-      <c r="N25" s="10">
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="N25" s="9">
         <v>672</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O25" s="9">
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="11">
-        <v>0</v>
-      </c>
-      <c r="D26" s="10">
-        <v>0</v>
-      </c>
-      <c r="E26" s="10">
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
         <v>1</v>
       </c>
       <c r="F26" s="1">
@@ -1845,10 +1842,10 @@
       <c r="G26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="9">
         <v>2782</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="9">
         <v>1826.24</v>
       </c>
       <c r="J26" s="1">
@@ -1857,30 +1854,30 @@
       <c r="K26" s="5">
         <v>0.98</v>
       </c>
-      <c r="L26" s="10">
-        <v>0</v>
-      </c>
-      <c r="N26" s="10">
+      <c r="L26" s="9">
+        <v>0</v>
+      </c>
+      <c r="N26" s="9">
         <v>672</v>
       </c>
-      <c r="O26" s="10">
+      <c r="O26" s="9">
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="11">
-        <v>0</v>
-      </c>
-      <c r="D27" s="10">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10">
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
         <v>1</v>
       </c>
       <c r="F27" s="1">
@@ -1889,10 +1886,10 @@
       <c r="G27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27" s="9">
         <v>1855</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="9">
         <v>1217.49</v>
       </c>
       <c r="J27" s="1">
@@ -1901,13 +1898,13 @@
       <c r="K27" s="5">
         <v>0.98</v>
       </c>
-      <c r="L27" s="10">
-        <v>0</v>
-      </c>
-      <c r="N27" s="10">
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
         <v>672</v>
       </c>
-      <c r="O27" s="10">
+      <c r="O27" s="9">
         <v>200</v>
       </c>
     </row>
@@ -1923,19 +1920,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA0D95F-4D73-4AC5-83CE-B4F9C15A7EF0}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1949,644 +1946,644 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <v>0.21724855683903974</v>
       </c>
       <c r="D2">
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>0.18410095683702996</v>
       </c>
       <c r="D3">
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>0.20520399948944013</v>
       </c>
       <c r="D4">
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>2.485003771776892</v>
       </c>
       <c r="D5">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>2.7412938262887514</v>
       </c>
       <c r="D6">
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>2.7193108053877015</v>
       </c>
       <c r="D7">
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="11">
         <v>2.8319946212158862</v>
       </c>
       <c r="D8">
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>2.9827126992277986</v>
       </c>
       <c r="D9">
         <v>4000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>3.048843702834902</v>
       </c>
       <c r="D10">
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>3.2857168797371226</v>
       </c>
       <c r="D11">
         <v>3900</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>3.0815801854075064</v>
       </c>
       <c r="D12">
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>3.5736669064789983</v>
       </c>
       <c r="D13">
         <v>3500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>0.30793000287983208</v>
       </c>
       <c r="D14">
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>0.288477808279203</v>
       </c>
       <c r="D15">
         <v>10000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="11">
         <v>0.3</v>
       </c>
       <c r="D16">
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="11">
         <v>0.06</v>
       </c>
       <c r="D17">
         <v>3600</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="11">
         <v>4.5088835074888228E-2</v>
       </c>
       <c r="D18">
         <v>2800</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="11">
         <v>0.04</v>
       </c>
       <c r="D19">
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="11">
         <v>0.05</v>
       </c>
       <c r="D20">
         <v>10000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="11">
         <v>4.2029070607330188E-2</v>
       </c>
       <c r="D21">
         <v>10000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>0.06</v>
       </c>
       <c r="D22">
         <v>10000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="11">
         <v>0.06</v>
       </c>
       <c r="D23">
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="11">
         <v>0.05</v>
       </c>
       <c r="D24">
         <v>5000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="11">
         <v>0.04</v>
       </c>
       <c r="D25">
         <v>3000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="11">
         <v>1.0556624603796714</v>
       </c>
       <c r="D26">
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="11">
         <v>1.0460012981166285</v>
       </c>
       <c r="D27">
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="11">
         <v>1.071009069983347</v>
       </c>
       <c r="D28">
         <v>2000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="11">
         <v>1.0501961198338507</v>
       </c>
       <c r="D29">
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="11">
         <v>1.1405813638643882</v>
       </c>
       <c r="D30">
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="11">
         <v>1.2461954609400137</v>
       </c>
       <c r="D31">
         <v>2000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="11">
         <v>1.2117538460834913</v>
       </c>
       <c r="D32">
         <v>3000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="11">
         <v>1.0964907284373231</v>
       </c>
       <c r="D33">
         <v>2500</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="11">
         <v>1.2847692671063502</v>
       </c>
       <c r="D34">
         <v>10000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="11">
         <v>1.4987265227537012</v>
       </c>
       <c r="D35">
         <v>10000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="13">
+      <c r="C36" s="11">
         <v>1.2831704495347027</v>
       </c>
       <c r="D36">
         <v>2000</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="11">
         <v>1.5270246300299162</v>
       </c>
       <c r="D37">
         <v>3000</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="11">
         <v>1.2437393891735411</v>
       </c>
       <c r="D38">
         <v>10000</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="13">
+      <c r="C39" s="11">
         <v>1.2336643552004152</v>
       </c>
       <c r="D39">
         <v>10000</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="13">
+      <c r="C40" s="11">
         <v>1.3268547049020489</v>
       </c>
       <c r="D40">
         <v>10000</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="11">
         <v>1.5066884814897361</v>
       </c>
       <c r="D41">
         <v>10000</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="11">
         <v>1.424362050193553</v>
       </c>
       <c r="D42">
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="11">
         <v>1.4489653010575458</v>
       </c>
       <c r="D43">
         <v>10000</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="11">
         <v>1.43</v>
       </c>
       <c r="D44">
         <v>10000</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="13">
+      <c r="C45" s="11">
         <v>1.5721616699539605</v>
       </c>
       <c r="D45">
         <v>10000</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="13">
+      <c r="C46" s="11">
         <v>2.5799923981434958</v>
       </c>
       <c r="D46">
         <v>10000</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="13">
+      <c r="C47" s="11">
         <v>2.6072703372574217</v>
       </c>
       <c r="D47">
@@ -2603,19 +2600,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66340080-EB6A-4DDF-B02B-0A061C261213}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2625,13 +2622,8 @@
       <c r="C1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2642,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2653,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -2664,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -2675,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -2686,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2697,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>